<commit_message>
Changes to the code: worksheet names, a new class created related to formatting excell spreadsheets
</commit_message>
<xml_diff>
--- a/DataAndResults.xlsx
+++ b/DataAndResults.xlsx
@@ -5,13 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="correct_login" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="test_login_results" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="other_test_results" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="DataForFacebookLogin" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TestResultsForFacebookLogin" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="other_test_results" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -33,12 +32,6 @@
   <si>
     <t xml:space="preserve">correct/incorrect</t>
   </si>
-  <si>
-    <t xml:space="preserve">correct password:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correct e-mail or username:</t>
-  </si>
 </sst>
 </file>
 
@@ -86,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -94,13 +87,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -127,7 +113,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -150,10 +136,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -183,8 +165,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -238,51 +220,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="25.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="3" width="9.14"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="6"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -294,11 +235,12 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
+    <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -310,23 +252,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="3" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="3" width="30"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -336,6 +282,14 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>